<commit_message>
refactor: make demo data more complete
</commit_message>
<xml_diff>
--- a/public/data/db-source/dataset.xlsx
+++ b/public/data/db-source/dataset.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11130"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/datannur/datannur_dev/public/data/db-source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB64E43A-4DF1-1B41-B2A7-FF0E5F754DFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14DAB604-B7ED-7245-8F80-954251BFB6B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="26740" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2440" yWindow="500" windowWidth="26360" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="225">
   <si>
     <t>id</t>
   </si>
@@ -334,12 +334,6 @@
     <t>tag_ids</t>
   </si>
   <si>
-    <t>personal_data, sensible_data, sante, population</t>
-  </si>
-  <si>
-    <t>anonymous_data, population, culture</t>
-  </si>
-  <si>
     <t>14-sante</t>
   </si>
   <si>
@@ -376,15 +370,6 @@
     <t>ofs-salaire</t>
   </si>
   <si>
-    <t>ofs-travail</t>
-  </si>
-  <si>
-    <t>ofs</t>
-  </si>
-  <si>
-    <t>ofs-tourisme</t>
-  </si>
-  <si>
     <t>ofs-div-pop</t>
   </si>
   <si>
@@ -457,10 +442,259 @@
     <t>Données sur l’emploi des jeunes de 18 à 36 ans</t>
   </si>
   <si>
-    <t>data/dataset/dataset-2.xlsx</t>
-  </si>
-  <si>
-    <t>pdf-wiki, pdf_online</t>
+    <t>theme_iso, securite, approvisionnement, anonymous_data</t>
+  </si>
+  <si>
+    <t>systemes_reference, armee, developpement_territorial</t>
+  </si>
+  <si>
+    <t>geologie, infrastructures, theme_iso, systemes_reference, sensible_data</t>
+  </si>
+  <si>
+    <t>infrastructures, images_aeriennes_2, edifices, cadastre_foncier, ouvrages, elimination</t>
+  </si>
+  <si>
+    <t>climatologie, personal_data, localisation, transport, faune, cadastre_foncier</t>
+  </si>
+  <si>
+    <t>sols, images_aeriennes_2</t>
+  </si>
+  <si>
+    <t>personal_data, data_protection, sensible_data, images_aeriennes_1</t>
+  </si>
+  <si>
+    <t>sols, localisation, altimetrie, pseudonymous_data, dangers_naturels, theme_iso</t>
+  </si>
+  <si>
+    <t>pseudonymous_data, transport, approvisionnement, infrastructures, theme_iso</t>
+  </si>
+  <si>
+    <t>sante, cadastre_foncier</t>
+  </si>
+  <si>
+    <t>dangers_naturels</t>
+  </si>
+  <si>
+    <t>securite, transport, personal_data, societe, elimination, systemes_reference</t>
+  </si>
+  <si>
+    <t>activites_economiques, flore</t>
+  </si>
+  <si>
+    <t>altimetrie, approvisionnement, armee, faune, images_aeriennes, culture</t>
+  </si>
+  <si>
+    <t>communication, anonymous_data, dangers_naturels, transport</t>
+  </si>
+  <si>
+    <t>ofs-mobi</t>
+  </si>
+  <si>
+    <t>ge-etat</t>
+  </si>
+  <si>
+    <t>ne-dfs</t>
+  </si>
+  <si>
+    <t>vd-etat</t>
+  </si>
+  <si>
+    <t>ofs-reg-ent</t>
+  </si>
+  <si>
+    <t>ofs-struct-eco</t>
+  </si>
+  <si>
+    <t>ge-df</t>
+  </si>
+  <si>
+    <t>dgaic</t>
+  </si>
+  <si>
+    <t>ne-etat</t>
+  </si>
+  <si>
+    <t>ofs-pop</t>
+  </si>
+  <si>
+    <t>suisse</t>
+  </si>
+  <si>
+    <t>vd-dgem</t>
+  </si>
+  <si>
+    <t>ofs-service-sante</t>
+  </si>
+  <si>
+    <t>dgnsi</t>
+  </si>
+  <si>
+    <t>profa</t>
+  </si>
+  <si>
+    <t>dac</t>
+  </si>
+  <si>
+    <t>dfa</t>
+  </si>
+  <si>
+    <t>vd-dge</t>
+  </si>
+  <si>
+    <t>avasad</t>
+  </si>
+  <si>
+    <t>dfjp</t>
+  </si>
+  <si>
+    <t>ofs-sys-form</t>
+  </si>
+  <si>
+    <t>vd-def</t>
+  </si>
+  <si>
+    <t>dcg</t>
+  </si>
+  <si>
+    <t>ofs-batiment</t>
+  </si>
+  <si>
+    <t>ofs-crim</t>
+  </si>
+  <si>
+    <t>camac</t>
+  </si>
+  <si>
+    <t>ofs-geo</t>
+  </si>
+  <si>
+    <t>https://statistique.admin.ch/view/ser-pub-loc</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/ofs-data/data/ser-pub-loc.csv</t>
+  </si>
+  <si>
+    <t>https://statistique.admin.ch/view/accident-route</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/ofs-data/data/accident-route.json</t>
+  </si>
+  <si>
+    <t>https://statistique.admin.ch/view/dep-sante</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/ofs-data/data/dep-sante.xlsx</t>
+  </si>
+  <si>
+    <t>https://opendata.swiss/view/temperature-moy</t>
+  </si>
+  <si>
+    <t>https://opendata.swiss/data/temperature-moy.parquet</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/ofs-data/view/pop-region</t>
+  </si>
+  <si>
+    <t>https://data.admin.ch/data/pop-region.json</t>
+  </si>
+  <si>
+    <t>https://opendata.swiss/view/eco-energies</t>
+  </si>
+  <si>
+    <t>https://opendata.swiss/data/eco-energies.parquet</t>
+  </si>
+  <si>
+    <t>https://opendata.swiss/data/eau-potable.json</t>
+  </si>
+  <si>
+    <t>https://opendata.swiss/view/tourisme-annu</t>
+  </si>
+  <si>
+    <t>https://data.admin.ch/data/tourisme-annu.parquet</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/ofs-data/view/pollution-air</t>
+  </si>
+  <si>
+    <t>https://data.admin.ch/data/pollution-air.csv</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/ofs-data/view/transport-pub</t>
+  </si>
+  <si>
+    <t>https://statistique.admin.ch/data/transport-pub.xlsx</t>
+  </si>
+  <si>
+    <t>https://statistique.admin.ch/view/usage-internet</t>
+  </si>
+  <si>
+    <t>https://statistique.admin.ch/view/emplois-tech</t>
+  </si>
+  <si>
+    <t>https://statistique.admin.ch/data/emplois-tech.xlsx</t>
+  </si>
+  <si>
+    <t>https://data.admin.ch/view/accidents-travail</t>
+  </si>
+  <si>
+    <t>https://opendata.swiss/data/accidents-travail.parquet</t>
+  </si>
+  <si>
+    <t>https://data.admin.ch/view/vente-voitures</t>
+  </si>
+  <si>
+    <t>https://opendata.swiss/data/vente-voitures.parquet</t>
+  </si>
+  <si>
+    <t>https://statistique.admin.ch/view/immobilier-prix</t>
+  </si>
+  <si>
+    <t>https://statistique.admin.ch/data/immobilier-prix.xlsx</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/ofs-data/view/conso-energie</t>
+  </si>
+  <si>
+    <t>https://data.admin.ch/data/conso-energie.xlsx</t>
+  </si>
+  <si>
+    <t>https://opendata.swiss/view/revenus-menages</t>
+  </si>
+  <si>
+    <t>https://data.admin.ch/data/revenus-menages.parquet</t>
+  </si>
+  <si>
+    <t>https://opendata.swiss/view/emploi-jeunes</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/ofs-data/data/emploi-jeunes.parquet</t>
+  </si>
+  <si>
+    <t>https://opendata.swiss/view/emplois-tech2</t>
+  </si>
+  <si>
+    <t>https://opendata.swiss/data/emplois-tech2.json</t>
+  </si>
+  <si>
+    <t>statpop-info</t>
+  </si>
+  <si>
+    <t>pdf-wiki</t>
+  </si>
+  <si>
+    <t>pdf_online, bevnat-variable</t>
+  </si>
+  <si>
+    <t>pdf-wiki, tourisme-exemple</t>
+  </si>
+  <si>
+    <t>bevnat-variable</t>
+  </si>
+  <si>
+    <t>statpop-info, tourisme-exemple</t>
+  </si>
+  <si>
+    <t>pop-com-1, pdf_online</t>
   </si>
 </sst>
 </file>
@@ -539,8 +773,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3C584991-6C49-624F-A55E-42748A4CF1EC}" name="Tableau1" displayName="Tableau1" ref="A1:S20" totalsRowShown="0">
-  <autoFilter ref="A1:S20" xr:uid="{3C584991-6C49-624F-A55E-42748A4CF1EC}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3C584991-6C49-624F-A55E-42748A4CF1EC}" name="Tableau1" displayName="Tableau1" ref="A1:S21" totalsRowShown="0">
+  <autoFilter ref="A1:S21" xr:uid="{3C584991-6C49-624F-A55E-42748A4CF1EC}"/>
   <tableColumns count="19">
     <tableColumn id="1" xr3:uid="{080E2F00-A22C-534D-B9C4-D8C8D5EB31DA}" name="id"/>
     <tableColumn id="2" xr3:uid="{92BFA972-4C1D-4E43-B990-63C7415BF3D0}" name="folder_id"/>
@@ -856,10 +1090,10 @@
   <dimension ref="A1:S21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="P2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S6" sqref="S6"/>
+      <selection pane="bottomRight" activeCell="S20" sqref="S20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -913,7 +1147,7 @@
         <v>9</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="K1" t="s">
         <v>10</v>
@@ -948,13 +1182,13 @@
         <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C2" t="s">
-        <v>119</v>
+        <v>155</v>
       </c>
       <c r="D2" t="s">
-        <v>120</v>
+        <v>156</v>
       </c>
       <c r="E2" t="s">
         <v>23</v>
@@ -969,7 +1203,7 @@
         <v>3000</v>
       </c>
       <c r="K2" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="L2" s="1">
         <v>2002</v>
@@ -982,6 +1216,15 @@
       </c>
       <c r="O2" t="s">
         <v>21</v>
+      </c>
+      <c r="P2" t="s">
+        <v>182</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>183</v>
+      </c>
+      <c r="R2" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
@@ -989,13 +1232,13 @@
         <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C3" t="s">
-        <v>119</v>
+        <v>157</v>
       </c>
       <c r="D3" t="s">
-        <v>121</v>
+        <v>158</v>
       </c>
       <c r="E3" t="s">
         <v>29</v>
@@ -1013,10 +1256,10 @@
         <v>33</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="K3" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>16</v>
@@ -1031,24 +1274,27 @@
         <v>20</v>
       </c>
       <c r="P3" t="s">
-        <v>145</v>
+        <v>184</v>
       </c>
       <c r="Q3" t="s">
-        <v>145</v>
+        <v>185</v>
+      </c>
+      <c r="R3" t="s">
+        <v>141</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C4" t="s">
-        <v>119</v>
+        <v>159</v>
       </c>
       <c r="D4" t="s">
-        <v>118</v>
+        <v>160</v>
       </c>
       <c r="E4" t="s">
         <v>34</v>
@@ -1066,7 +1312,7 @@
         <v>32</v>
       </c>
       <c r="K4" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -1076,11 +1322,14 @@
       <c r="O4" t="s">
         <v>21</v>
       </c>
+      <c r="P4" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>187</v>
+      </c>
       <c r="R4" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="S4" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
@@ -1088,7 +1337,13 @@
         <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>115</v>
+        <v>113</v>
+      </c>
+      <c r="C5" t="s">
+        <v>161</v>
+      </c>
+      <c r="D5" t="s">
+        <v>162</v>
       </c>
       <c r="E5" t="s">
         <v>36</v>
@@ -1097,7 +1352,7 @@
         <v>12</v>
       </c>
       <c r="G5" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="H5">
         <v>200</v>
@@ -1110,19 +1365,28 @@
       <c r="O5" t="s">
         <v>38</v>
       </c>
+      <c r="P5" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>189</v>
+      </c>
+      <c r="R5" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>39</v>
       </c>
       <c r="B6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C6" t="s">
-        <v>119</v>
+        <v>163</v>
       </c>
       <c r="D6" t="s">
-        <v>121</v>
+        <v>164</v>
       </c>
       <c r="E6" t="s">
         <v>40</v>
@@ -1131,7 +1395,7 @@
         <v>12</v>
       </c>
       <c r="G6" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="H6">
         <v>500000</v>
@@ -1140,7 +1404,7 @@
         <v>41</v>
       </c>
       <c r="K6" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>42</v>
@@ -1153,6 +1417,18 @@
       </c>
       <c r="O6" t="s">
         <v>21</v>
+      </c>
+      <c r="P6" t="s">
+        <v>190</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>191</v>
+      </c>
+      <c r="R6" t="s">
+        <v>144</v>
+      </c>
+      <c r="S6" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
@@ -1160,7 +1436,13 @@
         <v>44</v>
       </c>
       <c r="B7" t="s">
-        <v>107</v>
+        <v>105</v>
+      </c>
+      <c r="C7" t="s">
+        <v>165</v>
+      </c>
+      <c r="D7" t="s">
+        <v>166</v>
       </c>
       <c r="E7" t="s">
         <v>45</v>
@@ -1175,22 +1457,34 @@
         <v>47</v>
       </c>
       <c r="J7" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="K7" t="s">
+        <v>124</v>
+      </c>
+      <c r="L7" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="K7" t="s">
-        <v>129</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>140</v>
-      </c>
       <c r="M7" s="1" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="N7" t="s">
         <v>24</v>
       </c>
       <c r="O7" t="s">
         <v>20</v>
+      </c>
+      <c r="P7" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>193</v>
+      </c>
+      <c r="R7" t="s">
+        <v>145</v>
+      </c>
+      <c r="S7" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
@@ -1198,7 +1492,10 @@
         <v>48</v>
       </c>
       <c r="B8" t="s">
-        <v>106</v>
+        <v>104</v>
+      </c>
+      <c r="D8" t="s">
+        <v>167</v>
       </c>
       <c r="E8" t="s">
         <v>49</v>
@@ -1216,7 +1513,7 @@
         <v>51</v>
       </c>
       <c r="K8" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>52</v>
@@ -1229,6 +1526,12 @@
       </c>
       <c r="O8" t="s">
         <v>21</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>194</v>
+      </c>
+      <c r="S8" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
@@ -1236,13 +1539,13 @@
         <v>54</v>
       </c>
       <c r="B9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C9" t="s">
-        <v>119</v>
+        <v>168</v>
       </c>
       <c r="D9" t="s">
-        <v>120</v>
+        <v>165</v>
       </c>
       <c r="E9" t="s">
         <v>55</v>
@@ -1254,13 +1557,13 @@
         <v>56</v>
       </c>
       <c r="H9">
-        <v>320000</v>
+        <v>32389</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>57</v>
       </c>
       <c r="K9" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>58</v>
@@ -1273,6 +1576,15 @@
       </c>
       <c r="O9" t="s">
         <v>38</v>
+      </c>
+      <c r="P9" t="s">
+        <v>195</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>196</v>
+      </c>
+      <c r="R9" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
@@ -1280,6 +1592,9 @@
         <v>59</v>
       </c>
       <c r="B10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C10" t="s">
         <v>115</v>
       </c>
       <c r="E10" t="s">
@@ -1292,13 +1607,13 @@
         <v>61</v>
       </c>
       <c r="H10">
-        <v>67000</v>
+        <v>67050</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>62</v>
       </c>
       <c r="K10" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>63</v>
@@ -1311,6 +1626,15 @@
       </c>
       <c r="O10" t="s">
         <v>21</v>
+      </c>
+      <c r="P10" t="s">
+        <v>197</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>198</v>
+      </c>
+      <c r="R10" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
@@ -1318,7 +1642,13 @@
         <v>66</v>
       </c>
       <c r="B11" t="s">
-        <v>113</v>
+        <v>111</v>
+      </c>
+      <c r="C11" t="s">
+        <v>170</v>
+      </c>
+      <c r="D11" t="s">
+        <v>171</v>
       </c>
       <c r="E11" t="s">
         <v>67</v>
@@ -1327,16 +1657,16 @@
         <v>13</v>
       </c>
       <c r="G11" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="H11">
-        <v>999990</v>
+        <v>949563</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>68</v>
       </c>
       <c r="K11" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>69</v>
@@ -1349,6 +1679,15 @@
       </c>
       <c r="O11" t="s">
         <v>21</v>
+      </c>
+      <c r="P11" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>200</v>
+      </c>
+      <c r="R11" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
@@ -1356,7 +1695,13 @@
         <v>70</v>
       </c>
       <c r="B12" t="s">
-        <v>108</v>
+        <v>106</v>
+      </c>
+      <c r="C12" t="s">
+        <v>172</v>
+      </c>
+      <c r="D12" t="s">
+        <v>116</v>
       </c>
       <c r="E12" t="s">
         <v>71</v>
@@ -1374,13 +1719,13 @@
         <v>73</v>
       </c>
       <c r="K12" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>58</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="N12" t="s">
         <v>25</v>
@@ -1388,8 +1733,14 @@
       <c r="O12" t="s">
         <v>38</v>
       </c>
+      <c r="P12" t="s">
+        <v>201</v>
+      </c>
       <c r="R12" t="s">
-        <v>105</v>
+        <v>149</v>
+      </c>
+      <c r="S12" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.2">
@@ -1397,10 +1748,16 @@
         <v>74</v>
       </c>
       <c r="B13" t="s">
-        <v>109</v>
+        <v>107</v>
+      </c>
+      <c r="C13" t="s">
+        <v>173</v>
+      </c>
+      <c r="D13" t="s">
+        <v>157</v>
       </c>
       <c r="E13" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="F13" t="s">
         <v>13</v>
@@ -1409,25 +1766,34 @@
         <v>75</v>
       </c>
       <c r="H13">
-        <v>200000</v>
+        <v>45699</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>76</v>
       </c>
       <c r="K13" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>77</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="N13" t="s">
         <v>24</v>
       </c>
       <c r="O13" t="s">
         <v>21</v>
+      </c>
+      <c r="P13" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>203</v>
+      </c>
+      <c r="R13" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
@@ -1435,7 +1801,13 @@
         <v>78</v>
       </c>
       <c r="B14" t="s">
-        <v>106</v>
+        <v>104</v>
+      </c>
+      <c r="C14" t="s">
+        <v>174</v>
+      </c>
+      <c r="D14" t="s">
+        <v>169</v>
       </c>
       <c r="E14" t="s">
         <v>79</v>
@@ -1447,13 +1819,13 @@
         <v>80</v>
       </c>
       <c r="H14">
-        <v>85000</v>
+        <v>85005</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>81</v>
       </c>
       <c r="K14" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>52</v>
@@ -1466,6 +1838,15 @@
       </c>
       <c r="O14" t="s">
         <v>38</v>
+      </c>
+      <c r="P14" t="s">
+        <v>204</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>205</v>
+      </c>
+      <c r="S14" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.2">
@@ -1473,7 +1854,13 @@
         <v>82</v>
       </c>
       <c r="B15" t="s">
-        <v>113</v>
+        <v>111</v>
+      </c>
+      <c r="C15" t="s">
+        <v>164</v>
+      </c>
+      <c r="D15" t="s">
+        <v>115</v>
       </c>
       <c r="E15" t="s">
         <v>83</v>
@@ -1485,13 +1872,13 @@
         <v>84</v>
       </c>
       <c r="H15">
-        <v>99900</v>
+        <v>1144</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>85</v>
       </c>
       <c r="K15" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>69</v>
@@ -1504,6 +1891,12 @@
       </c>
       <c r="O15" t="s">
         <v>21</v>
+      </c>
+      <c r="P15" t="s">
+        <v>206</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
@@ -1511,7 +1904,7 @@
         <v>86</v>
       </c>
       <c r="B16" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E16" t="s">
         <v>87</v>
@@ -1523,13 +1916,13 @@
         <v>88</v>
       </c>
       <c r="H16">
-        <v>250000</v>
+        <v>44669</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>89</v>
       </c>
       <c r="K16" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>58</v>
@@ -1543,13 +1936,22 @@
       <c r="O16" t="s">
         <v>20</v>
       </c>
+      <c r="R16" t="s">
+        <v>151</v>
+      </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>90</v>
       </c>
       <c r="B17" t="s">
-        <v>111</v>
+        <v>109</v>
+      </c>
+      <c r="C17" t="s">
+        <v>175</v>
+      </c>
+      <c r="D17" t="s">
+        <v>176</v>
       </c>
       <c r="E17" t="s">
         <v>91</v>
@@ -1558,16 +1960,16 @@
         <v>12</v>
       </c>
       <c r="G17" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="H17">
-        <v>100000</v>
+        <v>75656</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>92</v>
       </c>
       <c r="K17" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="L17" s="1" t="s">
         <v>52</v>
@@ -1581,13 +1983,28 @@
       <c r="O17" t="s">
         <v>21</v>
       </c>
+      <c r="P17" t="s">
+        <v>208</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>209</v>
+      </c>
+      <c r="R17" t="s">
+        <v>152</v>
+      </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>93</v>
       </c>
       <c r="B18" t="s">
-        <v>110</v>
+        <v>108</v>
+      </c>
+      <c r="C18" t="s">
+        <v>177</v>
+      </c>
+      <c r="D18" t="s">
+        <v>165</v>
       </c>
       <c r="E18" t="s">
         <v>94</v>
@@ -1599,16 +2016,16 @@
         <v>95</v>
       </c>
       <c r="H18">
-        <v>1300000</v>
+        <v>434</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>68</v>
       </c>
       <c r="K18" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="M18" s="1" t="s">
         <v>43</v>
@@ -1619,19 +2036,31 @@
       <c r="O18" t="s">
         <v>38</v>
       </c>
+      <c r="P18" t="s">
+        <v>210</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>211</v>
+      </c>
+      <c r="R18" t="s">
+        <v>153</v>
+      </c>
+      <c r="S18" t="s">
+        <v>223</v>
+      </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>96</v>
       </c>
       <c r="B19" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C19" t="s">
-        <v>119</v>
+        <v>162</v>
       </c>
       <c r="D19" t="s">
-        <v>117</v>
+        <v>178</v>
       </c>
       <c r="E19" t="s">
         <v>97</v>
@@ -1643,19 +2072,19 @@
         <v>98</v>
       </c>
       <c r="H19">
-        <v>46000</v>
+        <v>47398</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="K19" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="L19" s="1" t="s">
         <v>52</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="N19" t="s">
         <v>65</v>
@@ -1663,37 +2092,49 @@
       <c r="O19" t="s">
         <v>21</v>
       </c>
+      <c r="P19" t="s">
+        <v>212</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>213</v>
+      </c>
+      <c r="R19" t="s">
+        <v>154</v>
+      </c>
+      <c r="S19" t="s">
+        <v>224</v>
+      </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>99</v>
       </c>
       <c r="B20" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C20" t="s">
-        <v>119</v>
+        <v>179</v>
       </c>
       <c r="D20" t="s">
-        <v>118</v>
+        <v>180</v>
       </c>
       <c r="E20" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="F20" t="s">
         <v>12</v>
       </c>
       <c r="G20" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="H20">
-        <v>100000</v>
+        <v>97344</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>100</v>
       </c>
       <c r="K20" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="L20" s="1" t="s">
         <v>101</v>
@@ -1707,16 +2148,31 @@
       <c r="O20" t="s">
         <v>21</v>
       </c>
+      <c r="P20" t="s">
+        <v>214</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>215</v>
+      </c>
+      <c r="R20" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B21" t="s">
-        <v>109</v>
+        <v>107</v>
+      </c>
+      <c r="C21" t="s">
+        <v>181</v>
+      </c>
+      <c r="D21" t="s">
+        <v>159</v>
       </c>
       <c r="E21" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="F21" t="s">
         <v>13</v>
@@ -1725,25 +2181,31 @@
         <v>75</v>
       </c>
       <c r="H21">
-        <v>200000</v>
+        <v>346</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="K21" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="L21" s="1" t="s">
         <v>77</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="N21" t="s">
         <v>24</v>
       </c>
       <c r="O21" t="s">
         <v>21</v>
+      </c>
+      <c r="P21" t="s">
+        <v>216</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>217</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor: make demo data more complete (#69)
</commit_message>
<xml_diff>
--- a/public/data/db-source/dataset.xlsx
+++ b/public/data/db-source/dataset.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11130"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/datannur/datannur_dev/public/data/db-source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB64E43A-4DF1-1B41-B2A7-FF0E5F754DFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14DAB604-B7ED-7245-8F80-954251BFB6B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="26740" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2440" yWindow="500" windowWidth="26360" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="225">
   <si>
     <t>id</t>
   </si>
@@ -334,12 +334,6 @@
     <t>tag_ids</t>
   </si>
   <si>
-    <t>personal_data, sensible_data, sante, population</t>
-  </si>
-  <si>
-    <t>anonymous_data, population, culture</t>
-  </si>
-  <si>
     <t>14-sante</t>
   </si>
   <si>
@@ -376,15 +370,6 @@
     <t>ofs-salaire</t>
   </si>
   <si>
-    <t>ofs-travail</t>
-  </si>
-  <si>
-    <t>ofs</t>
-  </si>
-  <si>
-    <t>ofs-tourisme</t>
-  </si>
-  <si>
     <t>ofs-div-pop</t>
   </si>
   <si>
@@ -457,10 +442,259 @@
     <t>Données sur l’emploi des jeunes de 18 à 36 ans</t>
   </si>
   <si>
-    <t>data/dataset/dataset-2.xlsx</t>
-  </si>
-  <si>
-    <t>pdf-wiki, pdf_online</t>
+    <t>theme_iso, securite, approvisionnement, anonymous_data</t>
+  </si>
+  <si>
+    <t>systemes_reference, armee, developpement_territorial</t>
+  </si>
+  <si>
+    <t>geologie, infrastructures, theme_iso, systemes_reference, sensible_data</t>
+  </si>
+  <si>
+    <t>infrastructures, images_aeriennes_2, edifices, cadastre_foncier, ouvrages, elimination</t>
+  </si>
+  <si>
+    <t>climatologie, personal_data, localisation, transport, faune, cadastre_foncier</t>
+  </si>
+  <si>
+    <t>sols, images_aeriennes_2</t>
+  </si>
+  <si>
+    <t>personal_data, data_protection, sensible_data, images_aeriennes_1</t>
+  </si>
+  <si>
+    <t>sols, localisation, altimetrie, pseudonymous_data, dangers_naturels, theme_iso</t>
+  </si>
+  <si>
+    <t>pseudonymous_data, transport, approvisionnement, infrastructures, theme_iso</t>
+  </si>
+  <si>
+    <t>sante, cadastre_foncier</t>
+  </si>
+  <si>
+    <t>dangers_naturels</t>
+  </si>
+  <si>
+    <t>securite, transport, personal_data, societe, elimination, systemes_reference</t>
+  </si>
+  <si>
+    <t>activites_economiques, flore</t>
+  </si>
+  <si>
+    <t>altimetrie, approvisionnement, armee, faune, images_aeriennes, culture</t>
+  </si>
+  <si>
+    <t>communication, anonymous_data, dangers_naturels, transport</t>
+  </si>
+  <si>
+    <t>ofs-mobi</t>
+  </si>
+  <si>
+    <t>ge-etat</t>
+  </si>
+  <si>
+    <t>ne-dfs</t>
+  </si>
+  <si>
+    <t>vd-etat</t>
+  </si>
+  <si>
+    <t>ofs-reg-ent</t>
+  </si>
+  <si>
+    <t>ofs-struct-eco</t>
+  </si>
+  <si>
+    <t>ge-df</t>
+  </si>
+  <si>
+    <t>dgaic</t>
+  </si>
+  <si>
+    <t>ne-etat</t>
+  </si>
+  <si>
+    <t>ofs-pop</t>
+  </si>
+  <si>
+    <t>suisse</t>
+  </si>
+  <si>
+    <t>vd-dgem</t>
+  </si>
+  <si>
+    <t>ofs-service-sante</t>
+  </si>
+  <si>
+    <t>dgnsi</t>
+  </si>
+  <si>
+    <t>profa</t>
+  </si>
+  <si>
+    <t>dac</t>
+  </si>
+  <si>
+    <t>dfa</t>
+  </si>
+  <si>
+    <t>vd-dge</t>
+  </si>
+  <si>
+    <t>avasad</t>
+  </si>
+  <si>
+    <t>dfjp</t>
+  </si>
+  <si>
+    <t>ofs-sys-form</t>
+  </si>
+  <si>
+    <t>vd-def</t>
+  </si>
+  <si>
+    <t>dcg</t>
+  </si>
+  <si>
+    <t>ofs-batiment</t>
+  </si>
+  <si>
+    <t>ofs-crim</t>
+  </si>
+  <si>
+    <t>camac</t>
+  </si>
+  <si>
+    <t>ofs-geo</t>
+  </si>
+  <si>
+    <t>https://statistique.admin.ch/view/ser-pub-loc</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/ofs-data/data/ser-pub-loc.csv</t>
+  </si>
+  <si>
+    <t>https://statistique.admin.ch/view/accident-route</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/ofs-data/data/accident-route.json</t>
+  </si>
+  <si>
+    <t>https://statistique.admin.ch/view/dep-sante</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/ofs-data/data/dep-sante.xlsx</t>
+  </si>
+  <si>
+    <t>https://opendata.swiss/view/temperature-moy</t>
+  </si>
+  <si>
+    <t>https://opendata.swiss/data/temperature-moy.parquet</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/ofs-data/view/pop-region</t>
+  </si>
+  <si>
+    <t>https://data.admin.ch/data/pop-region.json</t>
+  </si>
+  <si>
+    <t>https://opendata.swiss/view/eco-energies</t>
+  </si>
+  <si>
+    <t>https://opendata.swiss/data/eco-energies.parquet</t>
+  </si>
+  <si>
+    <t>https://opendata.swiss/data/eau-potable.json</t>
+  </si>
+  <si>
+    <t>https://opendata.swiss/view/tourisme-annu</t>
+  </si>
+  <si>
+    <t>https://data.admin.ch/data/tourisme-annu.parquet</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/ofs-data/view/pollution-air</t>
+  </si>
+  <si>
+    <t>https://data.admin.ch/data/pollution-air.csv</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/ofs-data/view/transport-pub</t>
+  </si>
+  <si>
+    <t>https://statistique.admin.ch/data/transport-pub.xlsx</t>
+  </si>
+  <si>
+    <t>https://statistique.admin.ch/view/usage-internet</t>
+  </si>
+  <si>
+    <t>https://statistique.admin.ch/view/emplois-tech</t>
+  </si>
+  <si>
+    <t>https://statistique.admin.ch/data/emplois-tech.xlsx</t>
+  </si>
+  <si>
+    <t>https://data.admin.ch/view/accidents-travail</t>
+  </si>
+  <si>
+    <t>https://opendata.swiss/data/accidents-travail.parquet</t>
+  </si>
+  <si>
+    <t>https://data.admin.ch/view/vente-voitures</t>
+  </si>
+  <si>
+    <t>https://opendata.swiss/data/vente-voitures.parquet</t>
+  </si>
+  <si>
+    <t>https://statistique.admin.ch/view/immobilier-prix</t>
+  </si>
+  <si>
+    <t>https://statistique.admin.ch/data/immobilier-prix.xlsx</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/ofs-data/view/conso-energie</t>
+  </si>
+  <si>
+    <t>https://data.admin.ch/data/conso-energie.xlsx</t>
+  </si>
+  <si>
+    <t>https://opendata.swiss/view/revenus-menages</t>
+  </si>
+  <si>
+    <t>https://data.admin.ch/data/revenus-menages.parquet</t>
+  </si>
+  <si>
+    <t>https://opendata.swiss/view/emploi-jeunes</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/ofs-data/data/emploi-jeunes.parquet</t>
+  </si>
+  <si>
+    <t>https://opendata.swiss/view/emplois-tech2</t>
+  </si>
+  <si>
+    <t>https://opendata.swiss/data/emplois-tech2.json</t>
+  </si>
+  <si>
+    <t>statpop-info</t>
+  </si>
+  <si>
+    <t>pdf-wiki</t>
+  </si>
+  <si>
+    <t>pdf_online, bevnat-variable</t>
+  </si>
+  <si>
+    <t>pdf-wiki, tourisme-exemple</t>
+  </si>
+  <si>
+    <t>bevnat-variable</t>
+  </si>
+  <si>
+    <t>statpop-info, tourisme-exemple</t>
+  </si>
+  <si>
+    <t>pop-com-1, pdf_online</t>
   </si>
 </sst>
 </file>
@@ -539,8 +773,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3C584991-6C49-624F-A55E-42748A4CF1EC}" name="Tableau1" displayName="Tableau1" ref="A1:S20" totalsRowShown="0">
-  <autoFilter ref="A1:S20" xr:uid="{3C584991-6C49-624F-A55E-42748A4CF1EC}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3C584991-6C49-624F-A55E-42748A4CF1EC}" name="Tableau1" displayName="Tableau1" ref="A1:S21" totalsRowShown="0">
+  <autoFilter ref="A1:S21" xr:uid="{3C584991-6C49-624F-A55E-42748A4CF1EC}"/>
   <tableColumns count="19">
     <tableColumn id="1" xr3:uid="{080E2F00-A22C-534D-B9C4-D8C8D5EB31DA}" name="id"/>
     <tableColumn id="2" xr3:uid="{92BFA972-4C1D-4E43-B990-63C7415BF3D0}" name="folder_id"/>
@@ -856,10 +1090,10 @@
   <dimension ref="A1:S21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="P2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S6" sqref="S6"/>
+      <selection pane="bottomRight" activeCell="S20" sqref="S20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -913,7 +1147,7 @@
         <v>9</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="K1" t="s">
         <v>10</v>
@@ -948,13 +1182,13 @@
         <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C2" t="s">
-        <v>119</v>
+        <v>155</v>
       </c>
       <c r="D2" t="s">
-        <v>120</v>
+        <v>156</v>
       </c>
       <c r="E2" t="s">
         <v>23</v>
@@ -969,7 +1203,7 @@
         <v>3000</v>
       </c>
       <c r="K2" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="L2" s="1">
         <v>2002</v>
@@ -982,6 +1216,15 @@
       </c>
       <c r="O2" t="s">
         <v>21</v>
+      </c>
+      <c r="P2" t="s">
+        <v>182</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>183</v>
+      </c>
+      <c r="R2" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
@@ -989,13 +1232,13 @@
         <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C3" t="s">
-        <v>119</v>
+        <v>157</v>
       </c>
       <c r="D3" t="s">
-        <v>121</v>
+        <v>158</v>
       </c>
       <c r="E3" t="s">
         <v>29</v>
@@ -1013,10 +1256,10 @@
         <v>33</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="K3" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>16</v>
@@ -1031,24 +1274,27 @@
         <v>20</v>
       </c>
       <c r="P3" t="s">
-        <v>145</v>
+        <v>184</v>
       </c>
       <c r="Q3" t="s">
-        <v>145</v>
+        <v>185</v>
+      </c>
+      <c r="R3" t="s">
+        <v>141</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C4" t="s">
-        <v>119</v>
+        <v>159</v>
       </c>
       <c r="D4" t="s">
-        <v>118</v>
+        <v>160</v>
       </c>
       <c r="E4" t="s">
         <v>34</v>
@@ -1066,7 +1312,7 @@
         <v>32</v>
       </c>
       <c r="K4" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -1076,11 +1322,14 @@
       <c r="O4" t="s">
         <v>21</v>
       </c>
+      <c r="P4" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>187</v>
+      </c>
       <c r="R4" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="S4" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
@@ -1088,7 +1337,13 @@
         <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>115</v>
+        <v>113</v>
+      </c>
+      <c r="C5" t="s">
+        <v>161</v>
+      </c>
+      <c r="D5" t="s">
+        <v>162</v>
       </c>
       <c r="E5" t="s">
         <v>36</v>
@@ -1097,7 +1352,7 @@
         <v>12</v>
       </c>
       <c r="G5" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="H5">
         <v>200</v>
@@ -1110,19 +1365,28 @@
       <c r="O5" t="s">
         <v>38</v>
       </c>
+      <c r="P5" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>189</v>
+      </c>
+      <c r="R5" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>39</v>
       </c>
       <c r="B6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C6" t="s">
-        <v>119</v>
+        <v>163</v>
       </c>
       <c r="D6" t="s">
-        <v>121</v>
+        <v>164</v>
       </c>
       <c r="E6" t="s">
         <v>40</v>
@@ -1131,7 +1395,7 @@
         <v>12</v>
       </c>
       <c r="G6" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="H6">
         <v>500000</v>
@@ -1140,7 +1404,7 @@
         <v>41</v>
       </c>
       <c r="K6" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>42</v>
@@ -1153,6 +1417,18 @@
       </c>
       <c r="O6" t="s">
         <v>21</v>
+      </c>
+      <c r="P6" t="s">
+        <v>190</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>191</v>
+      </c>
+      <c r="R6" t="s">
+        <v>144</v>
+      </c>
+      <c r="S6" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
@@ -1160,7 +1436,13 @@
         <v>44</v>
       </c>
       <c r="B7" t="s">
-        <v>107</v>
+        <v>105</v>
+      </c>
+      <c r="C7" t="s">
+        <v>165</v>
+      </c>
+      <c r="D7" t="s">
+        <v>166</v>
       </c>
       <c r="E7" t="s">
         <v>45</v>
@@ -1175,22 +1457,34 @@
         <v>47</v>
       </c>
       <c r="J7" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="K7" t="s">
+        <v>124</v>
+      </c>
+      <c r="L7" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="K7" t="s">
-        <v>129</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>140</v>
-      </c>
       <c r="M7" s="1" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="N7" t="s">
         <v>24</v>
       </c>
       <c r="O7" t="s">
         <v>20</v>
+      </c>
+      <c r="P7" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>193</v>
+      </c>
+      <c r="R7" t="s">
+        <v>145</v>
+      </c>
+      <c r="S7" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
@@ -1198,7 +1492,10 @@
         <v>48</v>
       </c>
       <c r="B8" t="s">
-        <v>106</v>
+        <v>104</v>
+      </c>
+      <c r="D8" t="s">
+        <v>167</v>
       </c>
       <c r="E8" t="s">
         <v>49</v>
@@ -1216,7 +1513,7 @@
         <v>51</v>
       </c>
       <c r="K8" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>52</v>
@@ -1229,6 +1526,12 @@
       </c>
       <c r="O8" t="s">
         <v>21</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>194</v>
+      </c>
+      <c r="S8" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
@@ -1236,13 +1539,13 @@
         <v>54</v>
       </c>
       <c r="B9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C9" t="s">
-        <v>119</v>
+        <v>168</v>
       </c>
       <c r="D9" t="s">
-        <v>120</v>
+        <v>165</v>
       </c>
       <c r="E9" t="s">
         <v>55</v>
@@ -1254,13 +1557,13 @@
         <v>56</v>
       </c>
       <c r="H9">
-        <v>320000</v>
+        <v>32389</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>57</v>
       </c>
       <c r="K9" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>58</v>
@@ -1273,6 +1576,15 @@
       </c>
       <c r="O9" t="s">
         <v>38</v>
+      </c>
+      <c r="P9" t="s">
+        <v>195</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>196</v>
+      </c>
+      <c r="R9" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
@@ -1280,6 +1592,9 @@
         <v>59</v>
       </c>
       <c r="B10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C10" t="s">
         <v>115</v>
       </c>
       <c r="E10" t="s">
@@ -1292,13 +1607,13 @@
         <v>61</v>
       </c>
       <c r="H10">
-        <v>67000</v>
+        <v>67050</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>62</v>
       </c>
       <c r="K10" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>63</v>
@@ -1311,6 +1626,15 @@
       </c>
       <c r="O10" t="s">
         <v>21</v>
+      </c>
+      <c r="P10" t="s">
+        <v>197</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>198</v>
+      </c>
+      <c r="R10" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
@@ -1318,7 +1642,13 @@
         <v>66</v>
       </c>
       <c r="B11" t="s">
-        <v>113</v>
+        <v>111</v>
+      </c>
+      <c r="C11" t="s">
+        <v>170</v>
+      </c>
+      <c r="D11" t="s">
+        <v>171</v>
       </c>
       <c r="E11" t="s">
         <v>67</v>
@@ -1327,16 +1657,16 @@
         <v>13</v>
       </c>
       <c r="G11" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="H11">
-        <v>999990</v>
+        <v>949563</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>68</v>
       </c>
       <c r="K11" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>69</v>
@@ -1349,6 +1679,15 @@
       </c>
       <c r="O11" t="s">
         <v>21</v>
+      </c>
+      <c r="P11" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>200</v>
+      </c>
+      <c r="R11" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
@@ -1356,7 +1695,13 @@
         <v>70</v>
       </c>
       <c r="B12" t="s">
-        <v>108</v>
+        <v>106</v>
+      </c>
+      <c r="C12" t="s">
+        <v>172</v>
+      </c>
+      <c r="D12" t="s">
+        <v>116</v>
       </c>
       <c r="E12" t="s">
         <v>71</v>
@@ -1374,13 +1719,13 @@
         <v>73</v>
       </c>
       <c r="K12" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>58</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="N12" t="s">
         <v>25</v>
@@ -1388,8 +1733,14 @@
       <c r="O12" t="s">
         <v>38</v>
       </c>
+      <c r="P12" t="s">
+        <v>201</v>
+      </c>
       <c r="R12" t="s">
-        <v>105</v>
+        <v>149</v>
+      </c>
+      <c r="S12" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.2">
@@ -1397,10 +1748,16 @@
         <v>74</v>
       </c>
       <c r="B13" t="s">
-        <v>109</v>
+        <v>107</v>
+      </c>
+      <c r="C13" t="s">
+        <v>173</v>
+      </c>
+      <c r="D13" t="s">
+        <v>157</v>
       </c>
       <c r="E13" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="F13" t="s">
         <v>13</v>
@@ -1409,25 +1766,34 @@
         <v>75</v>
       </c>
       <c r="H13">
-        <v>200000</v>
+        <v>45699</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>76</v>
       </c>
       <c r="K13" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>77</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="N13" t="s">
         <v>24</v>
       </c>
       <c r="O13" t="s">
         <v>21</v>
+      </c>
+      <c r="P13" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>203</v>
+      </c>
+      <c r="R13" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
@@ -1435,7 +1801,13 @@
         <v>78</v>
       </c>
       <c r="B14" t="s">
-        <v>106</v>
+        <v>104</v>
+      </c>
+      <c r="C14" t="s">
+        <v>174</v>
+      </c>
+      <c r="D14" t="s">
+        <v>169</v>
       </c>
       <c r="E14" t="s">
         <v>79</v>
@@ -1447,13 +1819,13 @@
         <v>80</v>
       </c>
       <c r="H14">
-        <v>85000</v>
+        <v>85005</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>81</v>
       </c>
       <c r="K14" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>52</v>
@@ -1466,6 +1838,15 @@
       </c>
       <c r="O14" t="s">
         <v>38</v>
+      </c>
+      <c r="P14" t="s">
+        <v>204</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>205</v>
+      </c>
+      <c r="S14" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.2">
@@ -1473,7 +1854,13 @@
         <v>82</v>
       </c>
       <c r="B15" t="s">
-        <v>113</v>
+        <v>111</v>
+      </c>
+      <c r="C15" t="s">
+        <v>164</v>
+      </c>
+      <c r="D15" t="s">
+        <v>115</v>
       </c>
       <c r="E15" t="s">
         <v>83</v>
@@ -1485,13 +1872,13 @@
         <v>84</v>
       </c>
       <c r="H15">
-        <v>99900</v>
+        <v>1144</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>85</v>
       </c>
       <c r="K15" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>69</v>
@@ -1504,6 +1891,12 @@
       </c>
       <c r="O15" t="s">
         <v>21</v>
+      </c>
+      <c r="P15" t="s">
+        <v>206</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
@@ -1511,7 +1904,7 @@
         <v>86</v>
       </c>
       <c r="B16" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E16" t="s">
         <v>87</v>
@@ -1523,13 +1916,13 @@
         <v>88</v>
       </c>
       <c r="H16">
-        <v>250000</v>
+        <v>44669</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>89</v>
       </c>
       <c r="K16" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>58</v>
@@ -1543,13 +1936,22 @@
       <c r="O16" t="s">
         <v>20</v>
       </c>
+      <c r="R16" t="s">
+        <v>151</v>
+      </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>90</v>
       </c>
       <c r="B17" t="s">
-        <v>111</v>
+        <v>109</v>
+      </c>
+      <c r="C17" t="s">
+        <v>175</v>
+      </c>
+      <c r="D17" t="s">
+        <v>176</v>
       </c>
       <c r="E17" t="s">
         <v>91</v>
@@ -1558,16 +1960,16 @@
         <v>12</v>
       </c>
       <c r="G17" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="H17">
-        <v>100000</v>
+        <v>75656</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>92</v>
       </c>
       <c r="K17" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="L17" s="1" t="s">
         <v>52</v>
@@ -1581,13 +1983,28 @@
       <c r="O17" t="s">
         <v>21</v>
       </c>
+      <c r="P17" t="s">
+        <v>208</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>209</v>
+      </c>
+      <c r="R17" t="s">
+        <v>152</v>
+      </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>93</v>
       </c>
       <c r="B18" t="s">
-        <v>110</v>
+        <v>108</v>
+      </c>
+      <c r="C18" t="s">
+        <v>177</v>
+      </c>
+      <c r="D18" t="s">
+        <v>165</v>
       </c>
       <c r="E18" t="s">
         <v>94</v>
@@ -1599,16 +2016,16 @@
         <v>95</v>
       </c>
       <c r="H18">
-        <v>1300000</v>
+        <v>434</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>68</v>
       </c>
       <c r="K18" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="M18" s="1" t="s">
         <v>43</v>
@@ -1619,19 +2036,31 @@
       <c r="O18" t="s">
         <v>38</v>
       </c>
+      <c r="P18" t="s">
+        <v>210</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>211</v>
+      </c>
+      <c r="R18" t="s">
+        <v>153</v>
+      </c>
+      <c r="S18" t="s">
+        <v>223</v>
+      </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>96</v>
       </c>
       <c r="B19" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C19" t="s">
-        <v>119</v>
+        <v>162</v>
       </c>
       <c r="D19" t="s">
-        <v>117</v>
+        <v>178</v>
       </c>
       <c r="E19" t="s">
         <v>97</v>
@@ -1643,19 +2072,19 @@
         <v>98</v>
       </c>
       <c r="H19">
-        <v>46000</v>
+        <v>47398</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="K19" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="L19" s="1" t="s">
         <v>52</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="N19" t="s">
         <v>65</v>
@@ -1663,37 +2092,49 @@
       <c r="O19" t="s">
         <v>21</v>
       </c>
+      <c r="P19" t="s">
+        <v>212</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>213</v>
+      </c>
+      <c r="R19" t="s">
+        <v>154</v>
+      </c>
+      <c r="S19" t="s">
+        <v>224</v>
+      </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>99</v>
       </c>
       <c r="B20" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C20" t="s">
-        <v>119</v>
+        <v>179</v>
       </c>
       <c r="D20" t="s">
-        <v>118</v>
+        <v>180</v>
       </c>
       <c r="E20" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="F20" t="s">
         <v>12</v>
       </c>
       <c r="G20" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="H20">
-        <v>100000</v>
+        <v>97344</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>100</v>
       </c>
       <c r="K20" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="L20" s="1" t="s">
         <v>101</v>
@@ -1707,16 +2148,31 @@
       <c r="O20" t="s">
         <v>21</v>
       </c>
+      <c r="P20" t="s">
+        <v>214</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>215</v>
+      </c>
+      <c r="R20" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B21" t="s">
-        <v>109</v>
+        <v>107</v>
+      </c>
+      <c r="C21" t="s">
+        <v>181</v>
+      </c>
+      <c r="D21" t="s">
+        <v>159</v>
       </c>
       <c r="E21" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="F21" t="s">
         <v>13</v>
@@ -1725,25 +2181,31 @@
         <v>75</v>
       </c>
       <c r="H21">
-        <v>200000</v>
+        <v>346</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="K21" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="L21" s="1" t="s">
         <v>77</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="N21" t="s">
         <v>24</v>
       </c>
       <c r="O21" t="s">
         <v>21</v>
+      </c>
+      <c r="P21" t="s">
+        <v>216</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>217</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: dataset link only for dataset with preview
</commit_message>
<xml_diff>
--- a/public/data/db-source/dataset.xlsx
+++ b/public/data/db-source/dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/datannur/datannur_dev/public/data/db-source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14DAB604-B7ED-7245-8F80-954251BFB6B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9262B4DA-1771-8744-82DE-8494BD335BB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2440" yWindow="500" windowWidth="26360" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="208">
   <si>
     <t>id</t>
   </si>
@@ -568,111 +568,57 @@
     <t>ofs-geo</t>
   </si>
   <si>
-    <t>https://statistique.admin.ch/view/ser-pub-loc</t>
-  </si>
-  <si>
     <t>https://raw.githubusercontent.com/ofs-data/data/ser-pub-loc.csv</t>
   </si>
   <si>
-    <t>https://statistique.admin.ch/view/accident-route</t>
-  </si>
-  <si>
     <t>https://raw.githubusercontent.com/ofs-data/data/accident-route.json</t>
   </si>
   <si>
-    <t>https://statistique.admin.ch/view/dep-sante</t>
-  </si>
-  <si>
     <t>https://raw.githubusercontent.com/ofs-data/data/dep-sante.xlsx</t>
   </si>
   <si>
-    <t>https://opendata.swiss/view/temperature-moy</t>
-  </si>
-  <si>
     <t>https://opendata.swiss/data/temperature-moy.parquet</t>
   </si>
   <si>
-    <t>https://raw.githubusercontent.com/ofs-data/view/pop-region</t>
-  </si>
-  <si>
     <t>https://data.admin.ch/data/pop-region.json</t>
   </si>
   <si>
-    <t>https://opendata.swiss/view/eco-energies</t>
-  </si>
-  <si>
     <t>https://opendata.swiss/data/eco-energies.parquet</t>
   </si>
   <si>
     <t>https://opendata.swiss/data/eau-potable.json</t>
   </si>
   <si>
-    <t>https://opendata.swiss/view/tourisme-annu</t>
-  </si>
-  <si>
     <t>https://data.admin.ch/data/tourisme-annu.parquet</t>
   </si>
   <si>
-    <t>https://raw.githubusercontent.com/ofs-data/view/pollution-air</t>
-  </si>
-  <si>
     <t>https://data.admin.ch/data/pollution-air.csv</t>
   </si>
   <si>
-    <t>https://raw.githubusercontent.com/ofs-data/view/transport-pub</t>
-  </si>
-  <si>
     <t>https://statistique.admin.ch/data/transport-pub.xlsx</t>
   </si>
   <si>
-    <t>https://statistique.admin.ch/view/usage-internet</t>
-  </si>
-  <si>
-    <t>https://statistique.admin.ch/view/emplois-tech</t>
-  </si>
-  <si>
     <t>https://statistique.admin.ch/data/emplois-tech.xlsx</t>
   </si>
   <si>
-    <t>https://data.admin.ch/view/accidents-travail</t>
-  </si>
-  <si>
     <t>https://opendata.swiss/data/accidents-travail.parquet</t>
   </si>
   <si>
-    <t>https://data.admin.ch/view/vente-voitures</t>
-  </si>
-  <si>
     <t>https://opendata.swiss/data/vente-voitures.parquet</t>
   </si>
   <si>
-    <t>https://statistique.admin.ch/view/immobilier-prix</t>
-  </si>
-  <si>
     <t>https://statistique.admin.ch/data/immobilier-prix.xlsx</t>
   </si>
   <si>
-    <t>https://raw.githubusercontent.com/ofs-data/view/conso-energie</t>
-  </si>
-  <si>
     <t>https://data.admin.ch/data/conso-energie.xlsx</t>
   </si>
   <si>
-    <t>https://opendata.swiss/view/revenus-menages</t>
-  </si>
-  <si>
     <t>https://data.admin.ch/data/revenus-menages.parquet</t>
   </si>
   <si>
-    <t>https://opendata.swiss/view/emploi-jeunes</t>
-  </si>
-  <si>
     <t>https://raw.githubusercontent.com/ofs-data/data/emploi-jeunes.parquet</t>
   </si>
   <si>
-    <t>https://opendata.swiss/view/emplois-tech2</t>
-  </si>
-  <si>
     <t>https://opendata.swiss/data/emplois-tech2.json</t>
   </si>
   <si>
@@ -695,6 +641,9 @@
   </si>
   <si>
     <t>pop-com-1, pdf_online</t>
+  </si>
+  <si>
+    <t>dataset/accident_route.xlsx</t>
   </si>
 </sst>
 </file>
@@ -1090,10 +1039,10 @@
   <dimension ref="A1:S21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S20" sqref="S20"/>
+      <selection pane="bottomRight" activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1217,11 +1166,8 @@
       <c r="O2" t="s">
         <v>21</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>182</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>183</v>
       </c>
       <c r="R2" t="s">
         <v>140</v>
@@ -1274,10 +1220,10 @@
         <v>20</v>
       </c>
       <c r="P3" t="s">
-        <v>184</v>
+        <v>207</v>
       </c>
       <c r="Q3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="R3" t="s">
         <v>141</v>
@@ -1322,11 +1268,8 @@
       <c r="O4" t="s">
         <v>21</v>
       </c>
-      <c r="P4" t="s">
-        <v>186</v>
-      </c>
       <c r="Q4" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="R4" s="2" t="s">
         <v>142</v>
@@ -1365,11 +1308,8 @@
       <c r="O5" t="s">
         <v>38</v>
       </c>
-      <c r="P5" t="s">
-        <v>188</v>
-      </c>
       <c r="Q5" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="R5" t="s">
         <v>143</v>
@@ -1418,17 +1358,14 @@
       <c r="O6" t="s">
         <v>21</v>
       </c>
-      <c r="P6" t="s">
-        <v>190</v>
-      </c>
       <c r="Q6" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="R6" t="s">
         <v>144</v>
       </c>
       <c r="S6" t="s">
-        <v>218</v>
+        <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
@@ -1474,17 +1411,14 @@
       <c r="O7" t="s">
         <v>20</v>
       </c>
-      <c r="P7" t="s">
-        <v>192</v>
-      </c>
       <c r="Q7" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="R7" t="s">
         <v>145</v>
       </c>
       <c r="S7" t="s">
-        <v>219</v>
+        <v>201</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
@@ -1528,10 +1462,10 @@
         <v>21</v>
       </c>
       <c r="Q8" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="S8" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
@@ -1577,11 +1511,8 @@
       <c r="O9" t="s">
         <v>38</v>
       </c>
-      <c r="P9" t="s">
-        <v>195</v>
-      </c>
       <c r="Q9" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="R9" t="s">
         <v>146</v>
@@ -1627,11 +1558,8 @@
       <c r="O10" t="s">
         <v>21</v>
       </c>
-      <c r="P10" t="s">
-        <v>197</v>
-      </c>
       <c r="Q10" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="R10" t="s">
         <v>147</v>
@@ -1680,11 +1608,8 @@
       <c r="O11" t="s">
         <v>21</v>
       </c>
-      <c r="P11" t="s">
-        <v>199</v>
-      </c>
       <c r="Q11" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="R11" t="s">
         <v>148</v>
@@ -1733,14 +1658,11 @@
       <c r="O12" t="s">
         <v>38</v>
       </c>
-      <c r="P12" t="s">
-        <v>201</v>
-      </c>
       <c r="R12" t="s">
         <v>149</v>
       </c>
       <c r="S12" t="s">
-        <v>221</v>
+        <v>203</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.2">
@@ -1786,11 +1708,8 @@
       <c r="O13" t="s">
         <v>21</v>
       </c>
-      <c r="P13" t="s">
-        <v>202</v>
-      </c>
       <c r="Q13" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="R13" t="s">
         <v>150</v>
@@ -1839,14 +1758,11 @@
       <c r="O14" t="s">
         <v>38</v>
       </c>
-      <c r="P14" t="s">
+      <c r="Q14" t="s">
+        <v>193</v>
+      </c>
+      <c r="S14" t="s">
         <v>204</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>205</v>
-      </c>
-      <c r="S14" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.2">
@@ -1892,11 +1808,8 @@
       <c r="O15" t="s">
         <v>21</v>
       </c>
-      <c r="P15" t="s">
-        <v>206</v>
-      </c>
       <c r="Q15" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
@@ -1983,11 +1896,8 @@
       <c r="O17" t="s">
         <v>21</v>
       </c>
-      <c r="P17" t="s">
-        <v>208</v>
-      </c>
       <c r="Q17" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
       <c r="R17" t="s">
         <v>152</v>
@@ -2036,17 +1946,14 @@
       <c r="O18" t="s">
         <v>38</v>
       </c>
-      <c r="P18" t="s">
-        <v>210</v>
-      </c>
       <c r="Q18" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
       <c r="R18" t="s">
         <v>153</v>
       </c>
       <c r="S18" t="s">
-        <v>223</v>
+        <v>205</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.2">
@@ -2092,17 +1999,14 @@
       <c r="O19" t="s">
         <v>21</v>
       </c>
-      <c r="P19" t="s">
-        <v>212</v>
-      </c>
       <c r="Q19" t="s">
-        <v>213</v>
+        <v>197</v>
       </c>
       <c r="R19" t="s">
         <v>154</v>
       </c>
       <c r="S19" t="s">
-        <v>224</v>
+        <v>206</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.2">
@@ -2148,11 +2052,8 @@
       <c r="O20" t="s">
         <v>21</v>
       </c>
-      <c r="P20" t="s">
-        <v>214</v>
-      </c>
       <c r="Q20" t="s">
-        <v>215</v>
+        <v>198</v>
       </c>
       <c r="R20" t="s">
         <v>11</v>
@@ -2201,11 +2102,8 @@
       <c r="O21" t="s">
         <v>21</v>
       </c>
-      <c r="P21" t="s">
-        <v>216</v>
-      </c>
       <c r="Q21" t="s">
-        <v>217</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add: LLM tab navigation and some little fixes (#75)
* fix: dataset link only for dataset with preview

* add: LLM tab navigation

* fix: change tab with LLM navigation in the same page

* fix: main scrollbar postion with chatPanel open
</commit_message>
<xml_diff>
--- a/public/data/db-source/dataset.xlsx
+++ b/public/data/db-source/dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/datannur/datannur_dev/public/data/db-source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14DAB604-B7ED-7245-8F80-954251BFB6B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9262B4DA-1771-8744-82DE-8494BD335BB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2440" yWindow="500" windowWidth="26360" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="208">
   <si>
     <t>id</t>
   </si>
@@ -568,111 +568,57 @@
     <t>ofs-geo</t>
   </si>
   <si>
-    <t>https://statistique.admin.ch/view/ser-pub-loc</t>
-  </si>
-  <si>
     <t>https://raw.githubusercontent.com/ofs-data/data/ser-pub-loc.csv</t>
   </si>
   <si>
-    <t>https://statistique.admin.ch/view/accident-route</t>
-  </si>
-  <si>
     <t>https://raw.githubusercontent.com/ofs-data/data/accident-route.json</t>
   </si>
   <si>
-    <t>https://statistique.admin.ch/view/dep-sante</t>
-  </si>
-  <si>
     <t>https://raw.githubusercontent.com/ofs-data/data/dep-sante.xlsx</t>
   </si>
   <si>
-    <t>https://opendata.swiss/view/temperature-moy</t>
-  </si>
-  <si>
     <t>https://opendata.swiss/data/temperature-moy.parquet</t>
   </si>
   <si>
-    <t>https://raw.githubusercontent.com/ofs-data/view/pop-region</t>
-  </si>
-  <si>
     <t>https://data.admin.ch/data/pop-region.json</t>
   </si>
   <si>
-    <t>https://opendata.swiss/view/eco-energies</t>
-  </si>
-  <si>
     <t>https://opendata.swiss/data/eco-energies.parquet</t>
   </si>
   <si>
     <t>https://opendata.swiss/data/eau-potable.json</t>
   </si>
   <si>
-    <t>https://opendata.swiss/view/tourisme-annu</t>
-  </si>
-  <si>
     <t>https://data.admin.ch/data/tourisme-annu.parquet</t>
   </si>
   <si>
-    <t>https://raw.githubusercontent.com/ofs-data/view/pollution-air</t>
-  </si>
-  <si>
     <t>https://data.admin.ch/data/pollution-air.csv</t>
   </si>
   <si>
-    <t>https://raw.githubusercontent.com/ofs-data/view/transport-pub</t>
-  </si>
-  <si>
     <t>https://statistique.admin.ch/data/transport-pub.xlsx</t>
   </si>
   <si>
-    <t>https://statistique.admin.ch/view/usage-internet</t>
-  </si>
-  <si>
-    <t>https://statistique.admin.ch/view/emplois-tech</t>
-  </si>
-  <si>
     <t>https://statistique.admin.ch/data/emplois-tech.xlsx</t>
   </si>
   <si>
-    <t>https://data.admin.ch/view/accidents-travail</t>
-  </si>
-  <si>
     <t>https://opendata.swiss/data/accidents-travail.parquet</t>
   </si>
   <si>
-    <t>https://data.admin.ch/view/vente-voitures</t>
-  </si>
-  <si>
     <t>https://opendata.swiss/data/vente-voitures.parquet</t>
   </si>
   <si>
-    <t>https://statistique.admin.ch/view/immobilier-prix</t>
-  </si>
-  <si>
     <t>https://statistique.admin.ch/data/immobilier-prix.xlsx</t>
   </si>
   <si>
-    <t>https://raw.githubusercontent.com/ofs-data/view/conso-energie</t>
-  </si>
-  <si>
     <t>https://data.admin.ch/data/conso-energie.xlsx</t>
   </si>
   <si>
-    <t>https://opendata.swiss/view/revenus-menages</t>
-  </si>
-  <si>
     <t>https://data.admin.ch/data/revenus-menages.parquet</t>
   </si>
   <si>
-    <t>https://opendata.swiss/view/emploi-jeunes</t>
-  </si>
-  <si>
     <t>https://raw.githubusercontent.com/ofs-data/data/emploi-jeunes.parquet</t>
   </si>
   <si>
-    <t>https://opendata.swiss/view/emplois-tech2</t>
-  </si>
-  <si>
     <t>https://opendata.swiss/data/emplois-tech2.json</t>
   </si>
   <si>
@@ -695,6 +641,9 @@
   </si>
   <si>
     <t>pop-com-1, pdf_online</t>
+  </si>
+  <si>
+    <t>dataset/accident_route.xlsx</t>
   </si>
 </sst>
 </file>
@@ -1090,10 +1039,10 @@
   <dimension ref="A1:S21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S20" sqref="S20"/>
+      <selection pane="bottomRight" activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1217,11 +1166,8 @@
       <c r="O2" t="s">
         <v>21</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>182</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>183</v>
       </c>
       <c r="R2" t="s">
         <v>140</v>
@@ -1274,10 +1220,10 @@
         <v>20</v>
       </c>
       <c r="P3" t="s">
-        <v>184</v>
+        <v>207</v>
       </c>
       <c r="Q3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="R3" t="s">
         <v>141</v>
@@ -1322,11 +1268,8 @@
       <c r="O4" t="s">
         <v>21</v>
       </c>
-      <c r="P4" t="s">
-        <v>186</v>
-      </c>
       <c r="Q4" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="R4" s="2" t="s">
         <v>142</v>
@@ -1365,11 +1308,8 @@
       <c r="O5" t="s">
         <v>38</v>
       </c>
-      <c r="P5" t="s">
-        <v>188</v>
-      </c>
       <c r="Q5" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="R5" t="s">
         <v>143</v>
@@ -1418,17 +1358,14 @@
       <c r="O6" t="s">
         <v>21</v>
       </c>
-      <c r="P6" t="s">
-        <v>190</v>
-      </c>
       <c r="Q6" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="R6" t="s">
         <v>144</v>
       </c>
       <c r="S6" t="s">
-        <v>218</v>
+        <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
@@ -1474,17 +1411,14 @@
       <c r="O7" t="s">
         <v>20</v>
       </c>
-      <c r="P7" t="s">
-        <v>192</v>
-      </c>
       <c r="Q7" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="R7" t="s">
         <v>145</v>
       </c>
       <c r="S7" t="s">
-        <v>219</v>
+        <v>201</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
@@ -1528,10 +1462,10 @@
         <v>21</v>
       </c>
       <c r="Q8" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="S8" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
@@ -1577,11 +1511,8 @@
       <c r="O9" t="s">
         <v>38</v>
       </c>
-      <c r="P9" t="s">
-        <v>195</v>
-      </c>
       <c r="Q9" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="R9" t="s">
         <v>146</v>
@@ -1627,11 +1558,8 @@
       <c r="O10" t="s">
         <v>21</v>
       </c>
-      <c r="P10" t="s">
-        <v>197</v>
-      </c>
       <c r="Q10" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="R10" t="s">
         <v>147</v>
@@ -1680,11 +1608,8 @@
       <c r="O11" t="s">
         <v>21</v>
       </c>
-      <c r="P11" t="s">
-        <v>199</v>
-      </c>
       <c r="Q11" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="R11" t="s">
         <v>148</v>
@@ -1733,14 +1658,11 @@
       <c r="O12" t="s">
         <v>38</v>
       </c>
-      <c r="P12" t="s">
-        <v>201</v>
-      </c>
       <c r="R12" t="s">
         <v>149</v>
       </c>
       <c r="S12" t="s">
-        <v>221</v>
+        <v>203</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.2">
@@ -1786,11 +1708,8 @@
       <c r="O13" t="s">
         <v>21</v>
       </c>
-      <c r="P13" t="s">
-        <v>202</v>
-      </c>
       <c r="Q13" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="R13" t="s">
         <v>150</v>
@@ -1839,14 +1758,11 @@
       <c r="O14" t="s">
         <v>38</v>
       </c>
-      <c r="P14" t="s">
+      <c r="Q14" t="s">
+        <v>193</v>
+      </c>
+      <c r="S14" t="s">
         <v>204</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>205</v>
-      </c>
-      <c r="S14" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.2">
@@ -1892,11 +1808,8 @@
       <c r="O15" t="s">
         <v>21</v>
       </c>
-      <c r="P15" t="s">
-        <v>206</v>
-      </c>
       <c r="Q15" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
@@ -1983,11 +1896,8 @@
       <c r="O17" t="s">
         <v>21</v>
       </c>
-      <c r="P17" t="s">
-        <v>208</v>
-      </c>
       <c r="Q17" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
       <c r="R17" t="s">
         <v>152</v>
@@ -2036,17 +1946,14 @@
       <c r="O18" t="s">
         <v>38</v>
       </c>
-      <c r="P18" t="s">
-        <v>210</v>
-      </c>
       <c r="Q18" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
       <c r="R18" t="s">
         <v>153</v>
       </c>
       <c r="S18" t="s">
-        <v>223</v>
+        <v>205</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.2">
@@ -2092,17 +1999,14 @@
       <c r="O19" t="s">
         <v>21</v>
       </c>
-      <c r="P19" t="s">
-        <v>212</v>
-      </c>
       <c r="Q19" t="s">
-        <v>213</v>
+        <v>197</v>
       </c>
       <c r="R19" t="s">
         <v>154</v>
       </c>
       <c r="S19" t="s">
-        <v>224</v>
+        <v>206</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.2">
@@ -2148,11 +2052,8 @@
       <c r="O20" t="s">
         <v>21</v>
       </c>
-      <c r="P20" t="s">
-        <v>214</v>
-      </c>
       <c r="Q20" t="s">
-        <v>215</v>
+        <v>198</v>
       </c>
       <c r="R20" t="s">
         <v>11</v>
@@ -2201,11 +2102,8 @@
       <c r="O21" t="s">
         <v>21</v>
       </c>
-      <c r="P21" t="s">
-        <v>216</v>
-      </c>
       <c r="Q21" t="s">
-        <v>217</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>

</xml_diff>